<commit_message>
Aanpassingen configuratie en template
</commit_message>
<xml_diff>
--- a/1. Configuratie.xlsx
+++ b/1. Configuratie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vrln.sharepoint.com/sites/GGD-ONDZ/PSchijf/Gezondheidsmonitor/Algemeen/Automatisering en R/Rapportage GMJ2023/Versie 10/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="156" documentId="8_{9135F566-5C0B-45DE-866D-BB2926EAD177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF9E928B-845E-4C7A-B68C-DB920289C75E}"/>
+  <xr:revisionPtr revIDLastSave="167" documentId="8_{9135F566-5C0B-45DE-866D-BB2926EAD177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36B2FAAE-2AE6-44B4-BA4E-36CDC738EC43}"/>
   <bookViews>
-    <workbookView xWindow="12" yWindow="12" windowWidth="23016" windowHeight="12336" xr2:uid="{340DDFAE-1A83-41FC-A379-531A17E4526A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{340DDFAE-1A83-41FC-A379-531A17E4526A}"/>
   </bookViews>
   <sheets>
     <sheet name="Rapportconfiguratie" sheetId="4" r:id="rId1"/>
@@ -41,8 +41,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={778CBD80-E1A3-47A0-B5C5-DC3E84201059}</author>
+  </authors>
+  <commentList>
+    <comment ref="D51" authorId="0" shapeId="0" xr:uid="{778CBD80-E1A3-47A0-B5C5-DC3E84201059}">
+      <text>
+        <t>[Opmerkingenthread]
+U kunt deze opmerkingenthread lezen in uw versie van Excel. Eventuele wijzigingen aan de thread gaan echter verloren als het bestand wordt geopend in een nieuwere versie van Excel. Meer informatie: https://go.microsoft.com/fwlink/?linkid=870924
+Opmerking:
+    Moet dit niet PBWBK3S2 zijn? (Is voldoende weerbaar)</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1243" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1243" uniqueCount="276">
   <si>
     <t>basis</t>
   </si>
@@ -531,9 +549,6 @@
   </si>
   <si>
     <t>Kan bij iemand terecht als hij/zij ergens mee zit</t>
-  </si>
-  <si>
-    <t>GBZOK3S17</t>
   </si>
   <si>
     <t>Percentage iemand terecht</t>
@@ -862,6 +877,18 @@
   </si>
   <si>
     <t>College van de Hoge Hoed</t>
+  </si>
+  <si>
+    <t>Is voldoende weerbaar</t>
+  </si>
+  <si>
+    <t>PBWBK3S2</t>
+  </si>
+  <si>
+    <t>Percentage weerbaar</t>
+  </si>
+  <si>
+    <t>GBZOK3S11</t>
   </si>
 </sst>
 </file>
@@ -971,7 +998,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1068,6 +1095,21 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1086,6 +1128,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Vermeulen, Sander" id="{DB7F9BFD-9AE8-413C-A685-3276F941A2CC}" userId="S::s.vermeulen@VRLN.NL::e08259fd-81d2-4a86-9b20-28ba02d67a18" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1383,11 +1431,19 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D51" dT="2024-01-24T08:21:15.02" personId="{DB7F9BFD-9AE8-413C-A685-3276F941A2CC}" id="{778CBD80-E1A3-47A0-B5C5-DC3E84201059}">
+    <text>Moet dit niet PBWBK3S2 zijn? (Is voldoende weerbaar)</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F0AA7A9-459B-4958-BBC2-94F84CFD8846}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1421,7 +1477,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>6</v>
@@ -1430,7 +1486,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -1441,10 +1497,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73A75041-D6C8-4C2F-941F-420EA079C5D1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73A75041-D6C8-4C2F-941F-420EA079C5D1}">
   <dimension ref="A1:L188"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1550,12 +1606,12 @@
       <c r="C4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>244</v>
+      <c r="D4" s="38" t="s">
+        <v>243</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -1821,7 +1877,7 @@
         <v>30</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>52</v>
@@ -1851,7 +1907,7 @@
         <v>55</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>52</v>
@@ -2189,7 +2245,7 @@
         <v>28</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>30</v>
@@ -2218,7 +2274,7 @@
         <v>28</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>30</v>
@@ -2282,7 +2338,7 @@
         <v>30</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E27" s="21" t="s">
         <v>52</v>
@@ -2311,7 +2367,7 @@
         <v>30</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E28" s="21" t="s">
         <v>52</v>
@@ -2404,7 +2460,7 @@
         <v>49</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>107</v>
@@ -2440,13 +2496,13 @@
         <v>55</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E32" s="21" t="s">
         <v>52</v>
       </c>
       <c r="F32" s="22" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I32" s="4" t="s">
         <v>0</v>
@@ -2507,7 +2563,7 @@
         <v>118</v>
       </c>
       <c r="E34" s="21" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I34" s="4" t="s">
         <v>81</v>
@@ -2527,13 +2583,13 @@
         <v>28</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>147</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E35" s="21" t="s">
         <v>52</v>
@@ -2548,7 +2604,7 @@
         <v>11</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
@@ -2909,13 +2965,13 @@
         <v>28</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>147</v>
       </c>
       <c r="D47" s="23" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E47" s="24" t="s">
         <v>52</v>
@@ -3026,64 +3082,64 @@
         <v>158</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A51" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="C51" s="4" t="s">
+    <row r="51" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="B51" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="C51" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="D51" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="E51" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F51" s="10"/>
-      <c r="I51" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="J51" s="4">
-        <v>2023</v>
-      </c>
-      <c r="K51" s="4">
+      <c r="D51" s="35" t="s">
+        <v>273</v>
+      </c>
+      <c r="E51" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="F51" s="37"/>
+      <c r="I51" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="J51" s="34">
+        <v>2023</v>
+      </c>
+      <c r="K51" s="34">
         <v>13</v>
       </c>
-      <c r="L51" s="4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A52" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B52" s="8" t="s">
+      <c r="L51" s="34" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="B52" s="35" t="s">
         <v>162</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="D52" s="8" t="s">
+      <c r="D52" s="35" t="s">
+        <v>275</v>
+      </c>
+      <c r="E52" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="F52" s="37"/>
+      <c r="I52" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="J52" s="34">
+        <v>2023</v>
+      </c>
+      <c r="K52" s="34">
+        <v>13</v>
+      </c>
+      <c r="L52" s="34" t="s">
         <v>163</v>
-      </c>
-      <c r="E52" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F52" s="10"/>
-      <c r="I52" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="J52" s="4">
-        <v>2023</v>
-      </c>
-      <c r="K52" s="4">
-        <v>13</v>
-      </c>
-      <c r="L52" s="4" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
@@ -3091,19 +3147,19 @@
         <v>28</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>88</v>
       </c>
       <c r="D53" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F53" s="10" t="s">
         <v>166</v>
-      </c>
-      <c r="E53" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F53" s="10" t="s">
-        <v>167</v>
       </c>
       <c r="H53" s="4" t="s">
         <v>63</v>
@@ -3118,7 +3174,7 @@
         <v>13</v>
       </c>
       <c r="L53" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
@@ -3126,16 +3182,16 @@
         <v>28</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>107</v>
       </c>
       <c r="D54" s="20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E54" s="21" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I54" s="4" t="s">
         <v>81</v>
@@ -3147,7 +3203,7 @@
         <v>13</v>
       </c>
       <c r="L54" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
@@ -3155,13 +3211,13 @@
         <v>28</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>147</v>
       </c>
       <c r="D55" s="23" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E55" s="24" t="s">
         <v>52</v>
@@ -3177,7 +3233,7 @@
         <v>14</v>
       </c>
       <c r="L55" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -3185,13 +3241,13 @@
         <v>28</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>147</v>
       </c>
       <c r="D56" s="23" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E56" s="24" t="s">
         <v>52</v>
@@ -3207,7 +3263,7 @@
         <v>14</v>
       </c>
       <c r="L56" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
@@ -3215,13 +3271,13 @@
         <v>28</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>61</v>
       </c>
       <c r="D57" s="15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E57" s="17" t="s">
         <v>52</v>
@@ -3243,7 +3299,7 @@
         <v>14</v>
       </c>
       <c r="L57" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="69" x14ac:dyDescent="0.3">
@@ -3251,19 +3307,19 @@
         <v>28</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>55</v>
       </c>
       <c r="D58" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="E58" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F58" s="16" t="s">
         <v>176</v>
-      </c>
-      <c r="E58" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F58" s="16" t="s">
-        <v>177</v>
       </c>
       <c r="I58" s="4" t="s">
         <v>0</v>
@@ -3275,7 +3331,7 @@
         <v>14</v>
       </c>
       <c r="L58" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
@@ -3283,13 +3339,13 @@
         <v>28</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>79</v>
       </c>
       <c r="D59" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E59" s="17" t="s">
         <v>52</v>
@@ -3305,7 +3361,7 @@
         <v>14</v>
       </c>
       <c r="L59" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="60" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
@@ -3313,19 +3369,19 @@
         <v>28</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>88</v>
       </c>
       <c r="D60" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F60" s="10" t="s">
         <v>183</v>
-      </c>
-      <c r="E60" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F60" s="10" t="s">
-        <v>184</v>
       </c>
       <c r="H60" s="4" t="s">
         <v>63</v>
@@ -3340,7 +3396,7 @@
         <v>14</v>
       </c>
       <c r="L60" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
@@ -3348,13 +3404,13 @@
         <v>28</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>79</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E61" s="9" t="s">
         <v>52</v>
@@ -3370,7 +3426,7 @@
         <v>15</v>
       </c>
       <c r="L61" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="62" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
@@ -3378,19 +3434,19 @@
         <v>28</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>55</v>
       </c>
       <c r="D62" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="E62" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F62" s="16" t="s">
         <v>190</v>
-      </c>
-      <c r="E62" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F62" s="16" t="s">
-        <v>191</v>
       </c>
       <c r="I62" s="4" t="s">
         <v>0</v>
@@ -3402,7 +3458,7 @@
         <v>15</v>
       </c>
       <c r="L62" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="63" spans="1:12" ht="96.6" x14ac:dyDescent="0.3">
@@ -3410,19 +3466,19 @@
         <v>28</v>
       </c>
       <c r="B63" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="C63" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="C63" s="4" t="s">
+      <c r="D63" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="D63" s="15" t="s">
+      <c r="E63" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F63" s="16" t="s">
         <v>195</v>
-      </c>
-      <c r="E63" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F63" s="16" t="s">
-        <v>196</v>
       </c>
       <c r="I63" s="4" t="s">
         <v>0</v>
@@ -3434,7 +3490,7 @@
         <v>15</v>
       </c>
       <c r="L63" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="64" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
@@ -3442,19 +3498,19 @@
         <v>28</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>88</v>
       </c>
       <c r="D64" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="E64" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F64" s="16" t="s">
         <v>199</v>
-      </c>
-      <c r="E64" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F64" s="16" t="s">
-        <v>200</v>
       </c>
       <c r="H64" s="4" t="s">
         <v>63</v>
@@ -3469,7 +3525,7 @@
         <v>15</v>
       </c>
       <c r="L64" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
@@ -3477,13 +3533,13 @@
         <v>28</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D65" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E65" s="17" t="s">
         <v>52</v>
@@ -3499,7 +3555,7 @@
         <v>16</v>
       </c>
       <c r="L65" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.3">
@@ -3507,13 +3563,13 @@
         <v>28</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D66" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E66" s="17" t="s">
         <v>52</v>
@@ -3529,7 +3585,7 @@
         <v>16</v>
       </c>
       <c r="L66" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
@@ -3537,13 +3593,13 @@
         <v>28</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D67" s="15" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E67" s="17" t="s">
         <v>52</v>
@@ -3559,7 +3615,7 @@
         <v>16</v>
       </c>
       <c r="L67" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
@@ -3567,13 +3623,13 @@
         <v>28</v>
       </c>
       <c r="B68" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D68" s="15" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E68" s="17" t="s">
         <v>52</v>
@@ -3589,7 +3645,7 @@
         <v>16</v>
       </c>
       <c r="L68" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
@@ -3597,13 +3653,13 @@
         <v>28</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>79</v>
       </c>
       <c r="D69" s="15" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E69" s="17" t="s">
         <v>52</v>
@@ -3619,7 +3675,7 @@
         <v>16</v>
       </c>
       <c r="L69" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="70" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
@@ -3627,19 +3683,19 @@
         <v>28</v>
       </c>
       <c r="B70" s="15" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>88</v>
       </c>
       <c r="D70" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="E70" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="F70" s="16" t="s">
         <v>214</v>
-      </c>
-      <c r="E70" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="F70" s="16" t="s">
-        <v>215</v>
       </c>
       <c r="H70" s="4" t="s">
         <v>63</v>
@@ -3654,7 +3710,7 @@
         <v>16</v>
       </c>
       <c r="L70" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.3">
@@ -3662,13 +3718,13 @@
         <v>28</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D71" s="15" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E71" s="16" t="s">
         <v>52</v>
@@ -3684,7 +3740,7 @@
         <v>16</v>
       </c>
       <c r="L71" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.3">
@@ -3692,13 +3748,13 @@
         <v>28</v>
       </c>
       <c r="B72" s="15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C72" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D72" s="15" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E72" s="16" t="s">
         <v>52</v>
@@ -3714,7 +3770,7 @@
         <v>16</v>
       </c>
       <c r="L72" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
@@ -3722,13 +3778,13 @@
         <v>28</v>
       </c>
       <c r="B73" s="15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>61</v>
       </c>
       <c r="D73" s="15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E73" s="16" t="s">
         <v>52</v>
@@ -3744,7 +3800,7 @@
         <v>17</v>
       </c>
       <c r="L73" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
@@ -3752,13 +3808,13 @@
         <v>28</v>
       </c>
       <c r="B74" s="15" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D74" s="15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E74" s="17" t="s">
         <v>52</v>
@@ -3774,7 +3830,7 @@
         <v>17</v>
       </c>
       <c r="L74" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.3">
@@ -3782,13 +3838,13 @@
         <v>28</v>
       </c>
       <c r="B75" s="15" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D75" s="15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E75" s="17" t="s">
         <v>52</v>
@@ -3804,7 +3860,7 @@
         <v>17</v>
       </c>
       <c r="L75" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.3">
@@ -3812,13 +3868,13 @@
         <v>28</v>
       </c>
       <c r="B76" s="15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D76" s="15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E76" s="17" t="s">
         <v>52</v>
@@ -3834,7 +3890,7 @@
         <v>17</v>
       </c>
       <c r="L76" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.3">
@@ -3842,13 +3898,13 @@
         <v>28</v>
       </c>
       <c r="B77" s="15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D77" s="15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E77" s="17" t="s">
         <v>52</v>
@@ -3864,7 +3920,7 @@
         <v>17</v>
       </c>
       <c r="L77" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.3">
@@ -3872,13 +3928,13 @@
         <v>28</v>
       </c>
       <c r="B78" s="15" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C78" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D78" s="15" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E78" s="17" t="s">
         <v>52</v>
@@ -3894,7 +3950,7 @@
         <v>17</v>
       </c>
       <c r="L78" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.3">
@@ -3902,13 +3958,13 @@
         <v>28</v>
       </c>
       <c r="B79" s="15" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C79" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D79" s="15" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E79" s="17" t="s">
         <v>52</v>
@@ -3924,7 +3980,7 @@
         <v>17</v>
       </c>
       <c r="L79" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="80" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
@@ -3932,19 +3988,19 @@
         <v>28</v>
       </c>
       <c r="B80" s="15" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C80" s="4" t="s">
         <v>88</v>
       </c>
       <c r="D80" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="E80" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="F80" s="16" t="s">
         <v>237</v>
-      </c>
-      <c r="E80" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="F80" s="16" t="s">
-        <v>238</v>
       </c>
       <c r="H80" s="4" t="s">
         <v>63</v>
@@ -3959,7 +4015,7 @@
         <v>17</v>
       </c>
       <c r="L80" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.3">
@@ -3967,13 +4023,13 @@
         <v>49</v>
       </c>
       <c r="B81" s="23" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C81" s="4" t="s">
         <v>107</v>
       </c>
       <c r="D81" s="26" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E81" s="21" t="s">
         <v>109</v>
@@ -3989,7 +4045,7 @@
         <v>18</v>
       </c>
       <c r="L81" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.3">
@@ -3997,13 +4053,13 @@
         <v>49</v>
       </c>
       <c r="B82" s="23" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C82" s="4" t="s">
         <v>107</v>
       </c>
       <c r="D82" s="26" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E82" s="21" t="s">
         <v>109</v>
@@ -4019,7 +4075,7 @@
         <v>18</v>
       </c>
       <c r="L82" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.3">
@@ -4636,6 +4692,7 @@
   <ignoredErrors>
     <ignoredError sqref="E13:E30 E33 E5:E9 E11 E53 E36:E39 E64 E57:E62 E49 E80 E76 E73:E74 E41:E44 E35 E45:E48 E75 E77:E79 E81:E82 E50:E52 E63 E65:E72 E40 E54:E56" numberStoredAsText="1"/>
   </ignoredErrors>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4750,11 +4807,11 @@
         <v>26</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -5388,7 +5445,7 @@
         <v>28</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>30</v>
@@ -5417,7 +5474,7 @@
         <v>28</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>30</v>
@@ -5481,7 +5538,7 @@
         <v>30</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E27" s="21" t="s">
         <v>52</v>
@@ -5510,7 +5567,7 @@
         <v>30</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E28" s="21" t="s">
         <v>52</v>
@@ -5603,7 +5660,7 @@
         <v>49</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>107</v>
@@ -5674,7 +5731,7 @@
         <v>118</v>
       </c>
       <c r="E33" s="21" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I33" s="4" t="s">
         <v>81</v>
@@ -5694,13 +5751,13 @@
         <v>28</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>147</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E34" s="24" t="s">
         <v>52</v>
@@ -5715,7 +5772,7 @@
         <v>11</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
@@ -6076,13 +6133,13 @@
         <v>28</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>147</v>
       </c>
       <c r="D46" s="23" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E46" s="24" t="s">
         <v>52</v>
@@ -6112,7 +6169,7 @@
         <v>55</v>
       </c>
       <c r="D47" s="30" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E47" s="24" t="s">
         <v>52</v>
@@ -6234,7 +6291,7 @@
         <v>30</v>
       </c>
       <c r="D51" s="31" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E51" s="9" t="s">
         <v>52</v>
@@ -6250,7 +6307,7 @@
         <v>13</v>
       </c>
       <c r="L51" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
@@ -6258,19 +6315,19 @@
         <v>28</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>88</v>
       </c>
       <c r="D52" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F52" s="10" t="s">
         <v>166</v>
-      </c>
-      <c r="E52" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F52" s="10" t="s">
-        <v>167</v>
       </c>
       <c r="H52" s="4" t="s">
         <v>63</v>
@@ -6285,7 +6342,7 @@
         <v>13</v>
       </c>
       <c r="L52" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
@@ -6293,16 +6350,16 @@
         <v>28</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>107</v>
       </c>
       <c r="D53" s="20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E53" s="21" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I53" s="4" t="s">
         <v>81</v>
@@ -6314,7 +6371,7 @@
         <v>13</v>
       </c>
       <c r="L53" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
@@ -6322,13 +6379,13 @@
         <v>28</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>147</v>
       </c>
       <c r="D54" s="23" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E54" s="24" t="s">
         <v>52</v>
@@ -6344,7 +6401,7 @@
         <v>14</v>
       </c>
       <c r="L54" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -6352,13 +6409,13 @@
         <v>28</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>147</v>
       </c>
       <c r="D55" s="23" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E55" s="24" t="s">
         <v>52</v>
@@ -6374,7 +6431,7 @@
         <v>14</v>
       </c>
       <c r="L55" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
@@ -6382,13 +6439,13 @@
         <v>28</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>61</v>
       </c>
       <c r="D56" s="15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E56" s="17" t="s">
         <v>52</v>
@@ -6410,7 +6467,7 @@
         <v>14</v>
       </c>
       <c r="L56" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="69" x14ac:dyDescent="0.3">
@@ -6418,19 +6475,19 @@
         <v>28</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>55</v>
       </c>
       <c r="D57" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="E57" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F57" s="16" t="s">
         <v>176</v>
-      </c>
-      <c r="E57" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F57" s="16" t="s">
-        <v>177</v>
       </c>
       <c r="I57" s="4" t="s">
         <v>0</v>
@@ -6442,7 +6499,7 @@
         <v>14</v>
       </c>
       <c r="L57" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
@@ -6450,13 +6507,13 @@
         <v>28</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>79</v>
       </c>
       <c r="D58" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E58" s="17" t="s">
         <v>52</v>
@@ -6472,7 +6529,7 @@
         <v>14</v>
       </c>
       <c r="L58" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
@@ -6480,19 +6537,19 @@
         <v>28</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>88</v>
       </c>
       <c r="D59" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="E59" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F59" s="10" t="s">
         <v>183</v>
-      </c>
-      <c r="E59" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F59" s="10" t="s">
-        <v>184</v>
       </c>
       <c r="H59" s="4" t="s">
         <v>63</v>
@@ -6507,7 +6564,7 @@
         <v>14</v>
       </c>
       <c r="L59" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
@@ -6515,13 +6572,13 @@
         <v>28</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>79</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E60" s="9" t="s">
         <v>52</v>
@@ -6537,7 +6594,7 @@
         <v>15</v>
       </c>
       <c r="L60" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="61" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
@@ -6545,19 +6602,19 @@
         <v>28</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>55</v>
       </c>
       <c r="D61" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="E61" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F61" s="16" t="s">
         <v>190</v>
-      </c>
-      <c r="E61" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F61" s="16" t="s">
-        <v>191</v>
       </c>
       <c r="I61" s="4" t="s">
         <v>0</v>
@@ -6569,7 +6626,7 @@
         <v>15</v>
       </c>
       <c r="L61" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="62" spans="1:12" ht="96.6" x14ac:dyDescent="0.3">
@@ -6577,19 +6634,19 @@
         <v>28</v>
       </c>
       <c r="B62" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="C62" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="D62" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="D62" s="15" t="s">
+      <c r="E62" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F62" s="16" t="s">
         <v>195</v>
-      </c>
-      <c r="E62" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F62" s="16" t="s">
-        <v>196</v>
       </c>
       <c r="I62" s="4" t="s">
         <v>0</v>
@@ -6601,7 +6658,7 @@
         <v>15</v>
       </c>
       <c r="L62" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="63" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
@@ -6609,19 +6666,19 @@
         <v>28</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>88</v>
       </c>
       <c r="D63" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="E63" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F63" s="16" t="s">
         <v>199</v>
-      </c>
-      <c r="E63" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F63" s="16" t="s">
-        <v>200</v>
       </c>
       <c r="H63" s="4" t="s">
         <v>63</v>
@@ -6636,7 +6693,7 @@
         <v>15</v>
       </c>
       <c r="L63" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
@@ -6644,13 +6701,13 @@
         <v>28</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D64" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E64" s="17" t="s">
         <v>52</v>
@@ -6666,7 +6723,7 @@
         <v>16</v>
       </c>
       <c r="L64" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
@@ -6674,13 +6731,13 @@
         <v>28</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D65" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E65" s="17" t="s">
         <v>52</v>
@@ -6696,7 +6753,7 @@
         <v>16</v>
       </c>
       <c r="L65" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.3">
@@ -6704,13 +6761,13 @@
         <v>28</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D66" s="15" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E66" s="17" t="s">
         <v>52</v>
@@ -6726,7 +6783,7 @@
         <v>16</v>
       </c>
       <c r="L66" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
@@ -6734,13 +6791,13 @@
         <v>28</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D67" s="15" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E67" s="17" t="s">
         <v>52</v>
@@ -6756,7 +6813,7 @@
         <v>16</v>
       </c>
       <c r="L67" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
@@ -6764,13 +6821,13 @@
         <v>28</v>
       </c>
       <c r="B68" s="15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>79</v>
       </c>
       <c r="D68" s="15" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E68" s="17" t="s">
         <v>52</v>
@@ -6786,7 +6843,7 @@
         <v>16</v>
       </c>
       <c r="L68" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="69" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
@@ -6794,19 +6851,19 @@
         <v>28</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>88</v>
       </c>
       <c r="D69" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="E69" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="F69" s="16" t="s">
         <v>214</v>
-      </c>
-      <c r="E69" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="F69" s="16" t="s">
-        <v>215</v>
       </c>
       <c r="H69" s="4" t="s">
         <v>63</v>
@@ -6821,7 +6878,7 @@
         <v>16</v>
       </c>
       <c r="L69" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.3">
@@ -6829,13 +6886,13 @@
         <v>28</v>
       </c>
       <c r="B70" s="15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D70" s="15" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E70" s="16" t="s">
         <v>52</v>
@@ -6851,7 +6908,7 @@
         <v>16</v>
       </c>
       <c r="L70" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.3">
@@ -6859,13 +6916,13 @@
         <v>28</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D71" s="15" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E71" s="16" t="s">
         <v>52</v>
@@ -6881,7 +6938,7 @@
         <v>16</v>
       </c>
       <c r="L71" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.3">
@@ -6889,13 +6946,13 @@
         <v>28</v>
       </c>
       <c r="B72" s="15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C72" s="4" t="s">
         <v>79</v>
       </c>
       <c r="D72" s="32" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E72" s="16" t="s">
         <v>52</v>
@@ -6911,7 +6968,7 @@
         <v>17</v>
       </c>
       <c r="L72" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
@@ -6919,13 +6976,13 @@
         <v>28</v>
       </c>
       <c r="B73" s="15" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D73" s="15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E73" s="17" t="s">
         <v>52</v>
@@ -6941,7 +6998,7 @@
         <v>17</v>
       </c>
       <c r="L73" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
@@ -6949,13 +7006,13 @@
         <v>28</v>
       </c>
       <c r="B74" s="15" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D74" s="15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E74" s="17" t="s">
         <v>52</v>
@@ -6971,7 +7028,7 @@
         <v>17</v>
       </c>
       <c r="L74" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.3">
@@ -6979,13 +7036,13 @@
         <v>28</v>
       </c>
       <c r="B75" s="15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D75" s="15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E75" s="17" t="s">
         <v>52</v>
@@ -7001,7 +7058,7 @@
         <v>17</v>
       </c>
       <c r="L75" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.3">
@@ -7009,13 +7066,13 @@
         <v>28</v>
       </c>
       <c r="B76" s="15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D76" s="15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E76" s="17" t="s">
         <v>52</v>
@@ -7031,7 +7088,7 @@
         <v>17</v>
       </c>
       <c r="L76" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.3">
@@ -7039,13 +7096,13 @@
         <v>28</v>
       </c>
       <c r="B77" s="15" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D77" s="15" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E77" s="17" t="s">
         <v>52</v>
@@ -7061,7 +7118,7 @@
         <v>17</v>
       </c>
       <c r="L77" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.3">
@@ -7069,13 +7126,13 @@
         <v>28</v>
       </c>
       <c r="B78" s="15" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C78" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D78" s="15" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E78" s="17" t="s">
         <v>52</v>
@@ -7091,7 +7148,7 @@
         <v>17</v>
       </c>
       <c r="L78" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="79" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
@@ -7099,19 +7156,19 @@
         <v>28</v>
       </c>
       <c r="B79" s="15" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C79" s="4" t="s">
         <v>88</v>
       </c>
       <c r="D79" s="32" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E79" s="17" t="s">
         <v>52</v>
       </c>
       <c r="F79" s="16" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H79" s="4" t="s">
         <v>63</v>
@@ -7126,7 +7183,7 @@
         <v>17</v>
       </c>
       <c r="L79" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.3">
@@ -7134,13 +7191,13 @@
         <v>49</v>
       </c>
       <c r="B80" s="23" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C80" s="4" t="s">
         <v>107</v>
       </c>
       <c r="D80" s="26" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E80" s="21" t="s">
         <v>109</v>
@@ -7156,7 +7213,7 @@
         <v>18</v>
       </c>
       <c r="L80" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.3">
@@ -7164,13 +7221,13 @@
         <v>49</v>
       </c>
       <c r="B81" s="23" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C81" s="4" t="s">
         <v>107</v>
       </c>
       <c r="D81" s="26" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E81" s="21" t="s">
         <v>109</v>
@@ -7186,7 +7243,7 @@
         <v>18</v>
       </c>
       <c r="L81" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.3">
@@ -7815,6 +7872,19 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4e95bed8-6d15-4403-ad70-a53422338dca">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C4EA295FB1FB9547A73C9F5819D6E613" ma:contentTypeVersion="20" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="26426b46a5c0c1d258bf284d595ef36f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="4e95bed8-6d15-4403-ad70-a53422338dca" xmlns:ns3="10d3344f-2d16-43d9-a145-97142f5cb288" xmlns:ns4="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7a995b3ef3034e03d49cf2989483892d" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -8091,19 +8161,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4e95bed8-6d15-4403-ad70-a53422338dca">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0EF40A6-8528-4994-A94E-1AE934020AF5}">
   <ds:schemaRefs>
@@ -8113,6 +8170,25 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFBB421F-7112-4B85-A662-9379706C03DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="c1085ce0-992b-4e2c-bc8b-9e7e29361dd3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="4e95bed8-6d15-4403-ad70-a53422338dca"/>
+    <ds:schemaRef ds:uri="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B7D56E5-F4DF-48D9-A1CD-EEB941D1E03B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8131,23 +8207,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFBB421F-7112-4B85-A662-9379706C03DC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="c1085ce0-992b-4e2c-bc8b-9e7e29361dd3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="4e95bed8-6d15-4403-ad70-a53422338dca"/>
-    <ds:schemaRef ds:uri="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
PBWBK3S7 aangepast naar PBWBK3S2
De indicator voor 'is voldoende weerbaar' stond nog verkeerd als PBWBK3S7 in de slideconfiguratie bij een combigrafiek, dit is nu aangepast naar PBWBK3S2
</commit_message>
<xml_diff>
--- a/1. Configuratie.xlsx
+++ b/1. Configuratie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vrln-my.sharepoint.com/personal/s_vermeulen_vrln_nl/Documents/Bureaublad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C11BA40-95A5-463C-825E-49E927D89F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C7AE25C-1F45-432D-8705-40A258EC101F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{340DDFAE-1A83-41FC-A379-531A17E4526A}"/>
   </bookViews>
@@ -39,24 +39,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={778CBD80-E1A3-47A0-B5C5-DC3E84201059}</author>
-  </authors>
-  <commentList>
-    <comment ref="D51" authorId="0" shapeId="0" xr:uid="{778CBD80-E1A3-47A0-B5C5-DC3E84201059}">
-      <text>
-        <t>[Opmerkingenthread]
-U kunt deze opmerkingenthread lezen in uw versie van Excel. Eventuele wijzigingen aan de thread gaan echter verloren als het bestand wordt geopend in een nieuwere versie van Excel. Meer informatie: https://go.microsoft.com/fwlink/?linkid=870924
-Opmerking:
-    Moet dit niet PBWBK3S2 zijn? (Is voldoende weerbaar)</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="267">
   <si>
@@ -537,9 +519,6 @@
     <t>Veerkracht</t>
   </si>
   <si>
-    <t>PBVKK3S2; PBVKK3S4; PBWBK3S7</t>
-  </si>
-  <si>
     <t>Herstelt snel; Moeilijk omgaan met stress; Goed voor zichzelf opkomen</t>
   </si>
   <si>
@@ -860,6 +839,9 @@
   </si>
   <si>
     <t>Slideconfiguratie 1</t>
+  </si>
+  <si>
+    <t>PBVKK3S2; PBVKK3S4; PBWBK3S2</t>
   </si>
 </sst>
 </file>
@@ -1069,9 +1051,7 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Vermeulen, Sander" id="{DB7F9BFD-9AE8-413C-A685-3276F941A2CC}" userId="S::s.vermeulen@VRLN.NL::e08259fd-81d2-4a86-9b20-28ba02d67a18" providerId="AD"/>
-</personList>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1369,14 +1349,6 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="D51" dT="2024-01-24T08:21:15.02" personId="{DB7F9BFD-9AE8-413C-A685-3276F941A2CC}" id="{778CBD80-E1A3-47A0-B5C5-DC3E84201059}">
-    <text>Moet dit niet PBWBK3S2 zijn? (Is voldoende weerbaar)</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F0AA7A9-459B-4958-BBC2-94F84CFD8846}">
   <dimension ref="A1:E2"/>
@@ -1415,7 +1387,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>6</v>
@@ -1424,7 +1396,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -1435,7 +1407,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73A75041-D6C8-4C2F-941F-420EA079C5D1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73A75041-D6C8-4C2F-941F-420EA079C5D1}">
   <dimension ref="A1:L188"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
@@ -1545,11 +1517,11 @@
         <v>26</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -1815,7 +1787,7 @@
         <v>30</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>51</v>
@@ -1845,7 +1817,7 @@
         <v>54</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>51</v>
@@ -2183,7 +2155,7 @@
         <v>28</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>30</v>
@@ -2212,7 +2184,7 @@
         <v>28</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>30</v>
@@ -2276,7 +2248,7 @@
         <v>30</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E27" s="21" t="s">
         <v>51</v>
@@ -2305,7 +2277,7 @@
         <v>30</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E28" s="21" t="s">
         <v>51</v>
@@ -2398,7 +2370,7 @@
         <v>49</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>105</v>
@@ -2434,13 +2406,13 @@
         <v>54</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E32" s="21" t="s">
         <v>51</v>
       </c>
       <c r="F32" s="22" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I32" s="4" t="s">
         <v>0</v>
@@ -2501,7 +2473,7 @@
         <v>116</v>
       </c>
       <c r="E34" s="21" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I34" s="4" t="s">
         <v>79</v>
@@ -2521,13 +2493,13 @@
         <v>28</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>144</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E35" s="21" t="s">
         <v>51</v>
@@ -2542,7 +2514,7 @@
         <v>11</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
@@ -2586,7 +2558,7 @@
         <v>30</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E37" s="9" t="s">
         <v>51</v>
@@ -2616,7 +2588,7 @@
         <v>30</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E38" s="9" t="s">
         <v>51</v>
@@ -2903,13 +2875,13 @@
         <v>28</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>144</v>
       </c>
       <c r="D47" s="23" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E47" s="24" t="s">
         <v>51</v>
@@ -3025,13 +2997,13 @@
         <v>28</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E51" s="9" t="s">
         <v>51</v>
@@ -3047,7 +3019,7 @@
         <v>13</v>
       </c>
       <c r="L51" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
@@ -3061,7 +3033,7 @@
         <v>30</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E52" s="9" t="s">
         <v>51</v>
@@ -3091,13 +3063,13 @@
         <v>86</v>
       </c>
       <c r="D53" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F53" s="10" t="s">
         <v>159</v>
-      </c>
-      <c r="E53" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="F53" s="10" t="s">
-        <v>160</v>
       </c>
       <c r="H53" s="4" t="s">
         <v>61</v>
@@ -3112,7 +3084,7 @@
         <v>13</v>
       </c>
       <c r="L53" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
@@ -3120,16 +3092,16 @@
         <v>28</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>105</v>
       </c>
       <c r="D54" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E54" s="21" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I54" s="4" t="s">
         <v>79</v>
@@ -3141,7 +3113,7 @@
         <v>13</v>
       </c>
       <c r="L54" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
@@ -3149,13 +3121,13 @@
         <v>28</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>144</v>
       </c>
       <c r="D55" s="23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E55" s="24" t="s">
         <v>51</v>
@@ -3171,7 +3143,7 @@
         <v>14</v>
       </c>
       <c r="L55" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -3179,13 +3151,13 @@
         <v>28</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>144</v>
       </c>
       <c r="D56" s="23" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E56" s="24" t="s">
         <v>51</v>
@@ -3201,7 +3173,7 @@
         <v>14</v>
       </c>
       <c r="L56" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
@@ -3209,13 +3181,13 @@
         <v>28</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>59</v>
       </c>
       <c r="D57" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E57" s="17" t="s">
         <v>51</v>
@@ -3237,7 +3209,7 @@
         <v>14</v>
       </c>
       <c r="L57" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="69" x14ac:dyDescent="0.3">
@@ -3245,19 +3217,19 @@
         <v>28</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>54</v>
       </c>
       <c r="D58" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="E58" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="F58" s="16" t="s">
         <v>169</v>
-      </c>
-      <c r="E58" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="F58" s="16" t="s">
-        <v>170</v>
       </c>
       <c r="I58" s="4" t="s">
         <v>0</v>
@@ -3269,7 +3241,7 @@
         <v>14</v>
       </c>
       <c r="L58" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
@@ -3277,13 +3249,13 @@
         <v>28</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>77</v>
       </c>
       <c r="D59" s="15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E59" s="17" t="s">
         <v>51</v>
@@ -3299,7 +3271,7 @@
         <v>14</v>
       </c>
       <c r="L59" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="60" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
@@ -3307,19 +3279,19 @@
         <v>28</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>86</v>
       </c>
       <c r="D60" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F60" s="10" t="s">
         <v>176</v>
-      </c>
-      <c r="E60" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="F60" s="10" t="s">
-        <v>177</v>
       </c>
       <c r="H60" s="4" t="s">
         <v>61</v>
@@ -3334,7 +3306,7 @@
         <v>14</v>
       </c>
       <c r="L60" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
@@ -3342,13 +3314,13 @@
         <v>28</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>77</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E61" s="9" t="s">
         <v>51</v>
@@ -3364,7 +3336,7 @@
         <v>15</v>
       </c>
       <c r="L61" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="62" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
@@ -3372,19 +3344,19 @@
         <v>28</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>54</v>
       </c>
       <c r="D62" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="E62" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="F62" s="16" t="s">
         <v>183</v>
-      </c>
-      <c r="E62" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="F62" s="16" t="s">
-        <v>184</v>
       </c>
       <c r="I62" s="4" t="s">
         <v>0</v>
@@ -3396,7 +3368,7 @@
         <v>15</v>
       </c>
       <c r="L62" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="63" spans="1:12" ht="96.6" x14ac:dyDescent="0.3">
@@ -3404,19 +3376,19 @@
         <v>28</v>
       </c>
       <c r="B63" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="C63" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C63" s="4" t="s">
+      <c r="D63" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="D63" s="15" t="s">
+      <c r="E63" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="F63" s="16" t="s">
         <v>188</v>
-      </c>
-      <c r="E63" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="F63" s="16" t="s">
-        <v>189</v>
       </c>
       <c r="I63" s="4" t="s">
         <v>0</v>
@@ -3428,7 +3400,7 @@
         <v>15</v>
       </c>
       <c r="L63" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="64" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
@@ -3436,19 +3408,19 @@
         <v>28</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>86</v>
       </c>
       <c r="D64" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="E64" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="F64" s="16" t="s">
         <v>192</v>
-      </c>
-      <c r="E64" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="F64" s="16" t="s">
-        <v>193</v>
       </c>
       <c r="H64" s="4" t="s">
         <v>61</v>
@@ -3463,7 +3435,7 @@
         <v>15</v>
       </c>
       <c r="L64" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
@@ -3471,13 +3443,13 @@
         <v>28</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D65" s="15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E65" s="17" t="s">
         <v>51</v>
@@ -3493,7 +3465,7 @@
         <v>16</v>
       </c>
       <c r="L65" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.3">
@@ -3501,13 +3473,13 @@
         <v>28</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D66" s="15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E66" s="17" t="s">
         <v>51</v>
@@ -3523,7 +3495,7 @@
         <v>16</v>
       </c>
       <c r="L66" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
@@ -3531,13 +3503,13 @@
         <v>28</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D67" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E67" s="17" t="s">
         <v>51</v>
@@ -3553,7 +3525,7 @@
         <v>16</v>
       </c>
       <c r="L67" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
@@ -3561,13 +3533,13 @@
         <v>28</v>
       </c>
       <c r="B68" s="15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D68" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E68" s="17" t="s">
         <v>51</v>
@@ -3583,7 +3555,7 @@
         <v>16</v>
       </c>
       <c r="L68" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
@@ -3591,13 +3563,13 @@
         <v>28</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>77</v>
       </c>
       <c r="D69" s="15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E69" s="17" t="s">
         <v>51</v>
@@ -3613,7 +3585,7 @@
         <v>16</v>
       </c>
       <c r="L69" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="70" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
@@ -3621,19 +3593,19 @@
         <v>28</v>
       </c>
       <c r="B70" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>86</v>
       </c>
       <c r="D70" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="E70" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="F70" s="16" t="s">
         <v>207</v>
-      </c>
-      <c r="E70" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="F70" s="16" t="s">
-        <v>208</v>
       </c>
       <c r="H70" s="4" t="s">
         <v>61</v>
@@ -3648,7 +3620,7 @@
         <v>16</v>
       </c>
       <c r="L70" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.3">
@@ -3656,13 +3628,13 @@
         <v>28</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D71" s="15" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E71" s="16" t="s">
         <v>51</v>
@@ -3678,7 +3650,7 @@
         <v>16</v>
       </c>
       <c r="L71" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.3">
@@ -3686,13 +3658,13 @@
         <v>28</v>
       </c>
       <c r="B72" s="15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C72" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D72" s="15" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E72" s="16" t="s">
         <v>51</v>
@@ -3708,7 +3680,7 @@
         <v>16</v>
       </c>
       <c r="L72" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
@@ -3716,13 +3688,13 @@
         <v>28</v>
       </c>
       <c r="B73" s="15" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>59</v>
       </c>
       <c r="D73" s="15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E73" s="16" t="s">
         <v>51</v>
@@ -3738,7 +3710,7 @@
         <v>17</v>
       </c>
       <c r="L73" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
@@ -3746,13 +3718,13 @@
         <v>28</v>
       </c>
       <c r="B74" s="15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D74" s="15" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E74" s="17" t="s">
         <v>51</v>
@@ -3768,7 +3740,7 @@
         <v>17</v>
       </c>
       <c r="L74" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.3">
@@ -3776,13 +3748,13 @@
         <v>28</v>
       </c>
       <c r="B75" s="15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D75" s="15" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E75" s="17" t="s">
         <v>51</v>
@@ -3798,7 +3770,7 @@
         <v>17</v>
       </c>
       <c r="L75" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.3">
@@ -3806,13 +3778,13 @@
         <v>28</v>
       </c>
       <c r="B76" s="15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D76" s="15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E76" s="17" t="s">
         <v>51</v>
@@ -3828,7 +3800,7 @@
         <v>17</v>
       </c>
       <c r="L76" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.3">
@@ -3836,13 +3808,13 @@
         <v>28</v>
       </c>
       <c r="B77" s="15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D77" s="15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E77" s="17" t="s">
         <v>51</v>
@@ -3858,7 +3830,7 @@
         <v>17</v>
       </c>
       <c r="L77" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.3">
@@ -3866,13 +3838,13 @@
         <v>28</v>
       </c>
       <c r="B78" s="15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C78" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D78" s="15" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E78" s="17" t="s">
         <v>51</v>
@@ -3888,7 +3860,7 @@
         <v>17</v>
       </c>
       <c r="L78" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.3">
@@ -3896,13 +3868,13 @@
         <v>28</v>
       </c>
       <c r="B79" s="15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C79" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D79" s="15" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E79" s="17" t="s">
         <v>51</v>
@@ -3918,7 +3890,7 @@
         <v>17</v>
       </c>
       <c r="L79" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="80" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
@@ -3926,19 +3898,19 @@
         <v>28</v>
       </c>
       <c r="B80" s="15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C80" s="4" t="s">
         <v>86</v>
       </c>
       <c r="D80" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="E80" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="F80" s="16" t="s">
         <v>230</v>
-      </c>
-      <c r="E80" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="F80" s="16" t="s">
-        <v>231</v>
       </c>
       <c r="H80" s="4" t="s">
         <v>61</v>
@@ -3953,7 +3925,7 @@
         <v>17</v>
       </c>
       <c r="L80" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.3">
@@ -3961,13 +3933,13 @@
         <v>49</v>
       </c>
       <c r="B81" s="23" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C81" s="4" t="s">
         <v>105</v>
       </c>
       <c r="D81" s="26" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E81" s="21" t="s">
         <v>107</v>
@@ -3983,7 +3955,7 @@
         <v>18</v>
       </c>
       <c r="L81" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.3">
@@ -3991,13 +3963,13 @@
         <v>49</v>
       </c>
       <c r="B82" s="23" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C82" s="4" t="s">
         <v>105</v>
       </c>
       <c r="D82" s="26" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E82" s="21" t="s">
         <v>107</v>
@@ -4013,7 +3985,7 @@
         <v>18</v>
       </c>
       <c r="L82" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.3">
@@ -4630,7 +4602,6 @@
   <ignoredErrors>
     <ignoredError sqref="E13:E30 E33 E5:E9 E11 E53 E36:E39 E64 E57:E62 E49 E80 E76 E73:E74 E41:E44 E35 E45:E48 E75 E77:E79 E81:E82 E50:E52 E63 E65:E72 E40 E54:E56" numberStoredAsText="1"/>
   </ignoredErrors>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4912,6 +4883,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -4922,15 +4902,6 @@
     <TaxCatchAll xmlns="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4955,6 +4926,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0EF40A6-8528-4994-A94E-1AE934020AF5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFBB421F-7112-4B85-A662-9379706C03DC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="c1085ce0-992b-4e2c-bc8b-9e7e29361dd3"/>
@@ -4971,12 +4950,4 @@
     <ds:schemaRef ds:uri="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0EF40A6-8528-4994-A94E-1AE934020AF5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>